<commit_message>
updated tests for push/pop vs PMA exceptions and haltreq during instruction excecution
Signed-off-by: Marton Teilgard <mateilga@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/debug-trace/CV32E40XS_debug.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/debug-trace/CV32E40XS_debug.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\openhw\core-v-verif_40s\cv32e40s\docs\VerifPlans\Simulation\debug-trace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E144C547-D266-4770-A942-BA1AC8DFB8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F74439-FD9C-40EE-83F5-0095B456355D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
@@ -2628,13 +2628,6 @@
     <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.umode_assert_i.a_mprven_tied</t>
   </si>
   <si>
-    <t>TODO: not covered</t>
-  </si>
-  <si>
-    <t>DTC: pushpop_debug_triggers
-TODO: Increase coverage by checking triggers at first/last operation</t>
-  </si>
-  <si>
     <t>A: [uvmt_cv32e40s_pmp_assert].a_accept_only_legal, [uvmt_cv32e40s_pmp_assert].a_deny_only_illegal</t>
   </si>
   <si>
@@ -2676,13 +2669,19 @@
   </si>
   <si>
     <t>This seems to be correct. And incorrect behaviour should therefore be triggered by the a_dt_store_trigger_hit_* assertions</t>
+  </si>
+  <si>
+    <t>Covered in DTC "debug_test2"</t>
+  </si>
+  <si>
+    <t>DTC: pushpop_debug_triggers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="48">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3118,7 +3117,7 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3203,31 +3202,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="6" borderId="2" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3236,20 +3235,14 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3747,11 +3740,11 @@
   <dimension ref="A1:M162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="6" customWidth="1"/>
@@ -3767,7 +3760,7 @@
     <col min="13" max="13" width="17" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -3808,20 +3801,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="93.75" customHeight="1">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:13" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="33" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="32" t="s">
@@ -3849,13 +3842,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="139.5" customHeight="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+    <row r="3" spans="1:13" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="10" t="s">
         <v>136</v>
       </c>
@@ -3878,23 +3871,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="142.15" customHeight="1">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:13" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="33" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -3919,13 +3912,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="142.15" customHeight="1">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+    <row r="5" spans="1:13" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="27" t="s">
         <v>136</v>
       </c>
@@ -3948,23 +3941,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="113.25" customHeight="1">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="42" t="s">
         <v>38</v>
       </c>
       <c r="G6" s="27" t="s">
@@ -3989,13 +3982,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="162.6" customHeight="1">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+    <row r="7" spans="1:13" ht="162.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="27" t="s">
         <v>136</v>
       </c>
@@ -4018,23 +4011,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="88.5" customHeight="1">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="42" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="27" t="s">
@@ -4059,13 +4052,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="147" customHeight="1">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+    <row r="9" spans="1:13" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="27" t="s">
         <v>136</v>
       </c>
@@ -4088,23 +4081,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="76.5" customHeight="1">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:13" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="38" t="s">
         <v>50</v>
       </c>
       <c r="G10" s="10" t="s">
@@ -4122,13 +4115,13 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="175.35" customHeight="1">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+    <row r="11" spans="1:13" ht="175.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="10" t="s">
         <v>136</v>
       </c>
@@ -4144,23 +4137,23 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G12" s="10" t="s">
@@ -4185,13 +4178,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="282" customHeight="1">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
+    <row r="13" spans="1:13" ht="282" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="10" t="s">
         <v>136</v>
       </c>
@@ -4214,17 +4207,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="61.5" customHeight="1">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:13" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="33" t="s">
         <v>56</v>
       </c>
       <c r="E14" s="32" t="s">
@@ -4250,11 +4243,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="88.35" customHeight="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+    <row r="15" spans="1:13" ht="88.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
       <c r="G15" s="10" t="s">
@@ -4272,23 +4265,23 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="80.25" customHeight="1">
-      <c r="A16" s="30" t="s">
+    <row r="16" spans="1:13" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="33" t="s">
         <v>69</v>
       </c>
       <c r="G16" s="10" t="s">
@@ -4313,13 +4306,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="43.5" customHeight="1">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
+    <row r="17" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="10" t="s">
         <v>136</v>
       </c>
@@ -4342,15 +4335,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="131.25" customHeight="1">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="36" t="s">
+    <row r="18" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="33" t="s">
         <v>73</v>
       </c>
       <c r="G18" s="10" t="s">
@@ -4375,13 +4368,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="131.25" customHeight="1">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="30"/>
+    <row r="19" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="33"/>
       <c r="G19" s="10" t="s">
         <v>136</v>
       </c>
@@ -4404,7 +4397,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="7" customFormat="1" ht="131.25" customHeight="1">
+    <row r="20" spans="1:13" s="7" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>76</v>
       </c>
@@ -4439,7 +4432,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" s="7" customFormat="1" ht="131.25" customHeight="1">
+    <row r="21" spans="1:13" s="7" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -4462,17 +4455,17 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="58.5" customHeight="1">
+    <row r="22" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="39"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="33" t="s">
         <v>84</v>
       </c>
       <c r="G22" s="10" t="s">
@@ -4497,13 +4490,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="58.5" customHeight="1">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
+    <row r="23" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="10" t="s">
         <v>136</v>
       </c>
@@ -4526,12 +4519,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="7" customFormat="1" ht="58.5" customHeight="1">
+    <row r="24" spans="1:13" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="32" t="s">
         <v>87</v>
       </c>
@@ -4554,10 +4547,10 @@
         <v>416</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="7" customFormat="1" ht="52.5" customHeight="1">
+    <row r="25" spans="1:13" s="7" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -4574,17 +4567,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="58.5" customHeight="1">
+    <row r="26" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="33" t="s">
         <v>93</v>
       </c>
       <c r="G26" s="10" t="s">
@@ -4609,13 +4602,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="58.5" customHeight="1">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
+    <row r="27" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="32"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="10" t="s">
         <v>136</v>
       </c>
@@ -4638,17 +4631,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="77.25" customHeight="1">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
+    <row r="28" spans="1:13" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="33" t="s">
         <v>96</v>
       </c>
       <c r="G28" s="10" t="s">
@@ -4673,13 +4666,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="65.25" customHeight="1">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
+    <row r="29" spans="1:13" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="32"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="10" t="s">
         <v>136</v>
       </c>
@@ -4702,7 +4695,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="7" customFormat="1" ht="105.75" customHeight="1">
+    <row r="30" spans="1:13" s="7" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="32"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -4737,13 +4730,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="7" customFormat="1" ht="65.25" customHeight="1">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="30"/>
+    <row r="31" spans="1:13" s="7" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="7" t="s">
         <v>136</v>
       </c>
@@ -4766,7 +4759,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="7" customFormat="1" ht="65.25" customHeight="1">
+    <row r="32" spans="1:13" s="7" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>76</v>
       </c>
@@ -4794,77 +4787,76 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="7" customFormat="1" ht="65.25" customHeight="1">
+    <row r="33" spans="1:13" s="7" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="F33" s="30" t="s">
         <v>427</v>
       </c>
-      <c r="E33" s="43" t="s">
+      <c r="G33" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="J33" s="31" t="s">
         <v>428</v>
       </c>
-      <c r="F33" s="44" t="s">
-        <v>429</v>
-      </c>
-      <c r="G33" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="H33" s="43" t="s">
-        <v>402</v>
-      </c>
-      <c r="I33" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="J33" s="45" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" s="7" customFormat="1" ht="65.25" customHeight="1">
+    </row>
+    <row r="34" spans="1:13" s="7" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="F34" s="42" t="s">
+      <c r="J34" s="31" t="s">
         <v>432</v>
       </c>
-      <c r="G34" s="42" t="s">
+    </row>
+    <row r="35" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="H34" s="43" t="s">
+      <c r="H35" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="I34" s="42" t="s">
-        <v>433</v>
-      </c>
-      <c r="J34" s="45" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="151.5" customHeight="1">
-      <c r="A35" s="10"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42" t="s">
+      <c r="I35" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="F35" s="42" t="s">
+      <c r="J35" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="G35" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="H35" s="43" t="s">
-        <v>402</v>
-      </c>
-      <c r="I35" s="42" t="s">
-        <v>437</v>
-      </c>
-      <c r="J35" s="45" t="s">
-        <v>438</v>
-      </c>
       <c r="K35" s="10" t="s">
         <v>23</v>
       </c>
@@ -4875,23 +4867,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="88.35" customHeight="1">
-      <c r="A36" s="30" t="s">
+    <row r="36" spans="1:13" ht="88.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="30" t="s">
+      <c r="E36" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="F36" s="30" t="s">
+      <c r="F36" s="33" t="s">
         <v>111</v>
       </c>
       <c r="G36" s="10" t="s">
@@ -4916,13 +4908,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="88.35" customHeight="1">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
+    <row r="37" spans="1:13" ht="88.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="10" t="s">
         <v>136</v>
       </c>
@@ -4945,17 +4937,17 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="51" customHeight="1">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30" t="s">
+    <row r="38" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="30" t="s">
+      <c r="F38" s="33" t="s">
         <v>116</v>
       </c>
       <c r="G38" s="10" t="s">
@@ -4980,13 +4972,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="50.25" customHeight="1">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
+    <row r="39" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
       <c r="G39" s="10" t="s">
         <v>136</v>
       </c>
@@ -5009,17 +5001,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="88.35" customHeight="1">
-      <c r="A40" s="30" t="s">
+    <row r="40" spans="1:13" ht="88.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="33" t="s">
         <v>119</v>
       </c>
       <c r="E40" s="32" t="s">
@@ -5050,11 +5042,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="88.35" customHeight="1">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
+    <row r="41" spans="1:13" ht="88.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
       <c r="E41" s="32"/>
       <c r="F41" s="32"/>
       <c r="G41" s="10" t="s">
@@ -5079,23 +5071,23 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="295.5" customHeight="1">
-      <c r="A42" s="30" t="s">
+    <row r="42" spans="1:13" ht="295.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="F42" s="30" t="s">
+      <c r="F42" s="33" t="s">
         <v>126</v>
       </c>
       <c r="G42" s="10" t="s">
@@ -5120,13 +5112,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="81" customHeight="1">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
+    <row r="43" spans="1:13" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
       <c r="G43" s="10" t="s">
         <v>136</v>
       </c>
@@ -5149,12 +5141,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="78.75" customHeight="1">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30" t="s">
+    <row r="44" spans="1:13" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33" t="s">
         <v>128</v>
       </c>
       <c r="F44" s="32" t="s">
@@ -5182,13 +5174,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="76.5" customHeight="1">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="33"/>
+    <row r="45" spans="1:13" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="43"/>
       <c r="G45" s="10" t="s">
         <v>136</v>
       </c>
@@ -5211,7 +5203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="76.5" customHeight="1">
+    <row r="46" spans="1:13" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>131</v>
       </c>
@@ -5244,21 +5236,21 @@
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" spans="1:13" ht="120" customHeight="1">
-      <c r="A47" s="30" t="s">
+    <row r="47" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30" t="s">
+      <c r="D47" s="33"/>
+      <c r="E47" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="F47" s="30" t="s">
+      <c r="F47" s="33" t="s">
         <v>141</v>
       </c>
       <c r="G47" s="10" t="s">
@@ -5280,13 +5272,13 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="159.75" customHeight="1">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
+    <row r="48" spans="1:13" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="33"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
       <c r="G48" s="10" t="s">
         <v>136</v>
       </c>
@@ -5302,23 +5294,23 @@
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
     </row>
-    <row r="49" spans="1:13" ht="42" customHeight="1">
-      <c r="A49" s="30" t="s">
+    <row r="49" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="30" t="s">
+      <c r="D49" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="E49" s="30" t="s">
+      <c r="E49" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="F49" s="30" t="s">
+      <c r="F49" s="33" t="s">
         <v>149</v>
       </c>
       <c r="G49" s="10" t="s">
@@ -5336,13 +5328,13 @@
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
     </row>
-    <row r="50" spans="1:13" ht="116.25" customHeight="1">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
+    <row r="50" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="33"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
       <c r="G50" s="10" t="s">
         <v>136</v>
       </c>
@@ -5358,7 +5350,7 @@
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
     </row>
-    <row r="51" spans="1:13" ht="78.75" customHeight="1">
+    <row r="51" spans="1:13" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>153</v>
       </c>
@@ -5397,23 +5389,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="242.25" customHeight="1">
-      <c r="A52" s="30" t="s">
+    <row r="52" spans="1:13" ht="242.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="30" t="s">
+      <c r="C52" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="D52" s="30" t="s">
+      <c r="D52" s="33" t="s">
         <v>159</v>
       </c>
       <c r="E52" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="F52" s="35" t="s">
+      <c r="F52" s="38" t="s">
         <v>161</v>
       </c>
       <c r="G52" s="10" t="s">
@@ -5438,13 +5430,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="210.75" customHeight="1">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
+    <row r="53" spans="1:13" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="33"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
       <c r="E53" s="32"/>
-      <c r="F53" s="30"/>
+      <c r="F53" s="33"/>
       <c r="G53" s="10" t="s">
         <v>136</v>
       </c>
@@ -5467,14 +5459,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="114" customHeight="1">
+    <row r="54" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="33" t="s">
         <v>158</v>
       </c>
       <c r="D54" s="10" t="s">
@@ -5508,7 +5500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="7" customFormat="1" ht="99" customHeight="1">
+    <row r="55" spans="1:13" s="7" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>170</v>
       </c>
@@ -5545,7 +5537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="7" customFormat="1" ht="84" customHeight="1">
+    <row r="56" spans="1:13" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>76</v>
       </c>
@@ -5573,7 +5565,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="7" customFormat="1" ht="59.25" customHeight="1">
+    <row r="57" spans="1:13" s="7" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>153</v>
       </c>
@@ -5610,7 +5602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="72.599999999999994" customHeight="1">
+    <row r="58" spans="1:13" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>181</v>
       </c>
@@ -5645,23 +5637,23 @@
       <c r="L58" s="10"/>
       <c r="M58" s="10"/>
     </row>
-    <row r="59" spans="1:13" ht="58.15" customHeight="1">
-      <c r="A59" s="34" t="s">
+    <row r="59" spans="1:13" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="C59" s="34" t="s">
+      <c r="C59" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="E59" s="34" t="s">
+      <c r="E59" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="F59" s="34" t="s">
+      <c r="F59" s="41" t="s">
         <v>191</v>
       </c>
       <c r="G59" s="17" t="s">
@@ -5675,13 +5667,13 @@
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
     </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="34"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="41"/>
+      <c r="B60" s="41"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
       <c r="G60" s="17" t="s">
         <v>25</v>
       </c>
@@ -5693,23 +5685,23 @@
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
     </row>
-    <row r="61" spans="1:13" ht="80.25" customHeight="1">
-      <c r="A61" s="30" t="s">
+    <row r="61" spans="1:13" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="C61" s="30" t="s">
+      <c r="C61" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E61" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="F61" s="30" t="s">
+      <c r="F61" s="33" t="s">
         <v>196</v>
       </c>
       <c r="G61" s="10" t="s">
@@ -5727,13 +5719,13 @@
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
     </row>
-    <row r="62" spans="1:13" ht="80.25" customHeight="1">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
+    <row r="62" spans="1:13" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="33"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
       <c r="G62" s="10" t="s">
         <v>25</v>
       </c>
@@ -5749,21 +5741,21 @@
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
     </row>
-    <row r="63" spans="1:13" ht="132.6" customHeight="1">
-      <c r="A63" s="30" t="s">
+    <row r="63" spans="1:13" ht="132.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B63" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="C63" s="30" t="s">
+      <c r="C63" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30" t="s">
+      <c r="D63" s="33"/>
+      <c r="E63" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="F63" s="30" t="s">
+      <c r="F63" s="33" t="s">
         <v>202</v>
       </c>
       <c r="G63" s="10" t="s">
@@ -5788,13 +5780,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="132.6" customHeight="1">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
+    <row r="64" spans="1:13" ht="132.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="33"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
       <c r="G64" s="10" t="s">
         <v>25</v>
       </c>
@@ -5817,7 +5809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="30">
+    <row r="65" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>181</v>
       </c>
@@ -5847,23 +5839,23 @@
         <v>211</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="72.599999999999994" customHeight="1">
-      <c r="A66" s="30" t="s">
+    <row r="66" spans="1:12" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="C66" s="30" t="s">
+      <c r="C66" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="D66" s="30" t="s">
+      <c r="D66" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="E66" s="30" t="s">
+      <c r="E66" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="F66" s="30" t="s">
+      <c r="F66" s="33" t="s">
         <v>215</v>
       </c>
       <c r="G66" s="10" t="s">
@@ -5881,13 +5873,13 @@
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
     </row>
-    <row r="67" spans="1:12" ht="67.5" customHeight="1">
-      <c r="A67" s="30"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
+    <row r="67" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="33"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="33"/>
       <c r="G67" s="10" t="s">
         <v>25</v>
       </c>
@@ -5903,23 +5895,23 @@
       <c r="K67" s="10"/>
       <c r="L67" s="10"/>
     </row>
-    <row r="68" spans="1:12" ht="109.15" customHeight="1">
-      <c r="A68" s="30" t="s">
+    <row r="68" spans="1:12" ht="109.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="C68" s="30" t="s">
+      <c r="C68" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D68" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="E68" s="35" t="s">
+      <c r="E68" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="F68" s="30" t="s">
+      <c r="F68" s="33" t="s">
         <v>221</v>
       </c>
       <c r="G68" s="10" t="s">
@@ -5937,13 +5929,13 @@
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
     </row>
-    <row r="69" spans="1:12" ht="109.15" customHeight="1">
-      <c r="A69" s="30"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
+    <row r="69" spans="1:12" ht="109.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="33"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="33"/>
       <c r="G69" s="10" t="s">
         <v>25</v>
       </c>
@@ -5959,7 +5951,7 @@
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
     </row>
-    <row r="70" spans="1:12" ht="236.45" customHeight="1">
+    <row r="70" spans="1:12" ht="236.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>181</v>
       </c>
@@ -5991,7 +5983,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="81.599999999999994" customHeight="1">
+    <row r="71" spans="1:12" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>181</v>
       </c>
@@ -6021,7 +6013,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="90.6" customHeight="1">
+    <row r="72" spans="1:12" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>181</v>
       </c>
@@ -6051,7 +6043,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="94.9" customHeight="1">
+    <row r="73" spans="1:12" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>181</v>
       </c>
@@ -6081,23 +6073,23 @@
         <v>211</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
-      <c r="A74" s="34" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="B74" s="41" t="s">
         <v>239</v>
       </c>
-      <c r="C74" s="34" t="s">
+      <c r="C74" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="D74" s="34" t="s">
+      <c r="D74" s="41" t="s">
         <v>240</v>
       </c>
-      <c r="E74" s="34" t="s">
+      <c r="E74" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="F74" s="34" t="s">
+      <c r="F74" s="41" t="s">
         <v>242</v>
       </c>
       <c r="G74" s="10"/>
@@ -6109,13 +6101,13 @@
       <c r="K74" s="10"/>
       <c r="L74" s="10"/>
     </row>
-    <row r="75" spans="1:12" ht="123.6" customHeight="1">
-      <c r="A75" s="34"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
+    <row r="75" spans="1:12" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="41"/>
+      <c r="B75" s="41"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="41"/>
+      <c r="E75" s="41"/>
+      <c r="F75" s="41"/>
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
@@ -6127,7 +6119,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="102" customHeight="1">
+    <row r="76" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
         <v>181</v>
       </c>
@@ -6151,23 +6143,23 @@
         <v>211</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="64.150000000000006" customHeight="1">
-      <c r="A77" s="30" t="s">
+    <row r="77" spans="1:12" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="C77" s="30" t="s">
+      <c r="C77" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D77" s="30" t="s">
+      <c r="D77" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="E77" s="30" t="s">
+      <c r="E77" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="F77" s="30" t="s">
+      <c r="F77" s="33" t="s">
         <v>248</v>
       </c>
       <c r="G77" s="10" t="s">
@@ -6187,13 +6179,13 @@
       </c>
       <c r="L77" s="10"/>
     </row>
-    <row r="78" spans="1:12" ht="64.150000000000006" customHeight="1">
-      <c r="A78" s="30"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="30"/>
+    <row r="78" spans="1:12" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="33"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="33"/>
+      <c r="F78" s="33"/>
       <c r="G78" s="10" t="s">
         <v>25</v>
       </c>
@@ -6209,23 +6201,23 @@
       <c r="K78" s="10"/>
       <c r="L78" s="10"/>
     </row>
-    <row r="79" spans="1:12" ht="109.9" customHeight="1">
-      <c r="A79" s="30" t="s">
+    <row r="79" spans="1:12" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="30" t="s">
+      <c r="B79" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="C79" s="30" t="s">
+      <c r="C79" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D79" s="30" t="s">
+      <c r="D79" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="E79" s="30" t="s">
+      <c r="E79" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="F79" s="30" t="s">
+      <c r="F79" s="33" t="s">
         <v>255</v>
       </c>
       <c r="G79" s="10" t="s">
@@ -6243,13 +6235,13 @@
       <c r="K79" s="10"/>
       <c r="L79" s="10"/>
     </row>
-    <row r="80" spans="1:12" ht="109.9" customHeight="1">
-      <c r="A80" s="30"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
+    <row r="80" spans="1:12" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="33"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="33"/>
       <c r="G80" s="10" t="s">
         <v>25</v>
       </c>
@@ -6265,23 +6257,23 @@
       <c r="K80" s="10"/>
       <c r="L80" s="10"/>
     </row>
-    <row r="81" spans="1:12" ht="94.9" customHeight="1">
-      <c r="A81" s="30" t="s">
+    <row r="81" spans="1:12" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B81" s="30" t="s">
+      <c r="B81" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="C81" s="30" t="s">
+      <c r="C81" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D81" s="30" t="s">
+      <c r="D81" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="E81" s="30" t="s">
+      <c r="E81" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="F81" s="30" t="s">
+      <c r="F81" s="33" t="s">
         <v>259</v>
       </c>
       <c r="G81" s="10" t="s">
@@ -6301,13 +6293,13 @@
       </c>
       <c r="L81" s="10"/>
     </row>
-    <row r="82" spans="1:12" ht="94.9" customHeight="1">
-      <c r="A82" s="30"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="30"/>
+    <row r="82" spans="1:12" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="33"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
       <c r="G82" s="10" t="s">
         <v>25</v>
       </c>
@@ -6323,23 +6315,23 @@
       <c r="K82" s="10"/>
       <c r="L82" s="10"/>
     </row>
-    <row r="83" spans="1:12" ht="141" customHeight="1">
-      <c r="A83" s="30" t="s">
+    <row r="83" spans="1:12" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B83" s="30" t="s">
+      <c r="B83" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="C83" s="30" t="s">
+      <c r="C83" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D83" s="30" t="s">
+      <c r="D83" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="E83" s="30" t="s">
+      <c r="E83" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="F83" s="30" t="s">
+      <c r="F83" s="33" t="s">
         <v>263</v>
       </c>
       <c r="G83" s="10" t="s">
@@ -6357,13 +6349,13 @@
       <c r="K83" s="10"/>
       <c r="L83" s="10"/>
     </row>
-    <row r="84" spans="1:12" ht="141" customHeight="1">
-      <c r="A84" s="30"/>
-      <c r="B84" s="30"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="30"/>
-      <c r="F84" s="30"/>
+    <row r="84" spans="1:12" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="33"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="33"/>
+      <c r="F84" s="33"/>
       <c r="G84" s="10" t="s">
         <v>25</v>
       </c>
@@ -6379,23 +6371,23 @@
       <c r="K84" s="10"/>
       <c r="L84" s="10"/>
     </row>
-    <row r="85" spans="1:12" ht="43.5" customHeight="1">
-      <c r="A85" s="30" t="s">
+    <row r="85" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B85" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="C85" s="34" t="s">
+      <c r="C85" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="D85" s="34" t="s">
+      <c r="D85" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="E85" s="34" t="s">
+      <c r="E85" s="41" t="s">
         <v>265</v>
       </c>
-      <c r="F85" s="34" t="s">
+      <c r="F85" s="41" t="s">
         <v>266</v>
       </c>
       <c r="G85" s="17" t="s">
@@ -6409,13 +6401,13 @@
       <c r="K85" s="10"/>
       <c r="L85" s="10"/>
     </row>
-    <row r="86" spans="1:12" ht="26.65" customHeight="1">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="34"/>
-      <c r="D86" s="34"/>
-      <c r="E86" s="34"/>
-      <c r="F86" s="34"/>
+    <row r="86" spans="1:12" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="33"/>
+      <c r="B86" s="33"/>
+      <c r="C86" s="41"/>
+      <c r="D86" s="41"/>
+      <c r="E86" s="41"/>
+      <c r="F86" s="41"/>
       <c r="G86" s="17" t="s">
         <v>25</v>
       </c>
@@ -6427,20 +6419,20 @@
       <c r="K86" s="10"/>
       <c r="L86" s="10"/>
     </row>
-    <row r="87" spans="1:12" ht="58.15" customHeight="1">
-      <c r="A87" s="30" t="s">
+    <row r="87" spans="1:12" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B87" s="30" t="s">
+      <c r="B87" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="C87" s="30" t="s">
+      <c r="C87" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D87" s="30" t="s">
+      <c r="D87" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="E87" s="30" t="s">
+      <c r="E87" s="33" t="s">
         <v>267</v>
       </c>
       <c r="F87" s="32" t="s">
@@ -6461,13 +6453,13 @@
       <c r="K87" s="10"/>
       <c r="L87" s="10"/>
     </row>
-    <row r="88" spans="1:12" ht="75">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="30"/>
+    <row r="88" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A88" s="33"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
       <c r="G88" s="10" t="s">
         <v>25</v>
       </c>
@@ -6483,23 +6475,23 @@
       <c r="K88" s="10"/>
       <c r="L88" s="10"/>
     </row>
-    <row r="89" spans="1:12" ht="43.5" customHeight="1">
-      <c r="A89" s="30" t="s">
+    <row r="89" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B89" s="30" t="s">
+      <c r="B89" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="C89" s="30" t="s">
+      <c r="C89" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D89" s="30" t="s">
+      <c r="D89" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="E89" s="30" t="s">
+      <c r="E89" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="F89" s="30" t="s">
+      <c r="F89" s="33" t="s">
         <v>271</v>
       </c>
       <c r="G89" s="10" t="s">
@@ -6517,13 +6509,13 @@
       <c r="K89" s="10"/>
       <c r="L89" s="10"/>
     </row>
-    <row r="90" spans="1:12" ht="60">
-      <c r="A90" s="30"/>
-      <c r="B90" s="30"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="30"/>
+    <row r="90" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A90" s="33"/>
+      <c r="B90" s="33"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="33"/>
       <c r="G90" s="10" t="s">
         <v>25</v>
       </c>
@@ -6539,23 +6531,23 @@
       <c r="K90" s="10"/>
       <c r="L90" s="10"/>
     </row>
-    <row r="91" spans="1:12" ht="43.5" customHeight="1">
-      <c r="A91" s="30" t="s">
+    <row r="91" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B91" s="30" t="s">
+      <c r="B91" s="33" t="s">
         <v>273</v>
       </c>
-      <c r="C91" s="30" t="s">
+      <c r="C91" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D91" s="30" t="s">
+      <c r="D91" s="33" t="s">
         <v>274</v>
       </c>
-      <c r="E91" s="30" t="s">
+      <c r="E91" s="33" t="s">
         <v>275</v>
       </c>
-      <c r="F91" s="30" t="s">
+      <c r="F91" s="33" t="s">
         <v>276</v>
       </c>
       <c r="G91" s="10" t="s">
@@ -6573,13 +6565,13 @@
       <c r="K91" s="10"/>
       <c r="L91" s="10"/>
     </row>
-    <row r="92" spans="1:12" ht="60">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="30"/>
+    <row r="92" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A92" s="33"/>
+      <c r="B92" s="33"/>
+      <c r="C92" s="33"/>
+      <c r="D92" s="33"/>
+      <c r="E92" s="33"/>
+      <c r="F92" s="33"/>
       <c r="G92" s="10" t="s">
         <v>25</v>
       </c>
@@ -6595,23 +6587,23 @@
       <c r="K92" s="10"/>
       <c r="L92" s="10"/>
     </row>
-    <row r="93" spans="1:12" ht="43.5" customHeight="1">
-      <c r="A93" s="30" t="s">
+    <row r="93" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B93" s="30" t="s">
+      <c r="B93" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="C93" s="30" t="s">
+      <c r="C93" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D93" s="30" t="s">
+      <c r="D93" s="33" t="s">
         <v>280</v>
       </c>
-      <c r="E93" s="30" t="s">
+      <c r="E93" s="33" t="s">
         <v>281</v>
       </c>
-      <c r="F93" s="30" t="s">
+      <c r="F93" s="33" t="s">
         <v>282</v>
       </c>
       <c r="G93" s="10" t="s">
@@ -6629,13 +6621,13 @@
       <c r="K93" s="10"/>
       <c r="L93" s="10"/>
     </row>
-    <row r="94" spans="1:12" ht="60">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
+    <row r="94" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94" s="33"/>
+      <c r="B94" s="33"/>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="33"/>
+      <c r="F94" s="33"/>
       <c r="G94" s="10" t="s">
         <v>25</v>
       </c>
@@ -6651,23 +6643,23 @@
       <c r="K94" s="10"/>
       <c r="L94" s="10"/>
     </row>
-    <row r="95" spans="1:12" ht="54.75" customHeight="1">
-      <c r="A95" s="30" t="s">
+    <row r="95" spans="1:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B95" s="30" t="s">
+      <c r="B95" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="C95" s="30" t="s">
+      <c r="C95" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D95" s="30" t="s">
+      <c r="D95" s="33" t="s">
         <v>280</v>
       </c>
-      <c r="E95" s="30" t="s">
+      <c r="E95" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="F95" s="30" t="s">
+      <c r="F95" s="33" t="s">
         <v>286</v>
       </c>
       <c r="G95" s="10" t="s">
@@ -6687,13 +6679,13 @@
       </c>
       <c r="L95" s="10"/>
     </row>
-    <row r="96" spans="1:12" ht="75.75" customHeight="1">
-      <c r="A96" s="30"/>
-      <c r="B96" s="30"/>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="30"/>
-      <c r="F96" s="30"/>
+    <row r="96" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="33"/>
+      <c r="B96" s="33"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33"/>
       <c r="G96" s="10" t="s">
         <v>25</v>
       </c>
@@ -6709,23 +6701,23 @@
       <c r="K96" s="10"/>
       <c r="L96" s="10"/>
     </row>
-    <row r="97" spans="1:13" ht="75.75" customHeight="1">
-      <c r="A97" s="30" t="s">
+    <row r="97" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B97" s="30" t="s">
+      <c r="B97" s="33" t="s">
         <v>290</v>
       </c>
-      <c r="C97" s="30" t="s">
+      <c r="C97" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D97" s="30" t="s">
+      <c r="D97" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="E97" s="30" t="s">
+      <c r="E97" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="F97" s="30" t="s">
+      <c r="F97" s="33" t="s">
         <v>293</v>
       </c>
       <c r="G97" s="10" t="s">
@@ -6750,13 +6742,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="75.75" customHeight="1">
-      <c r="A98" s="30"/>
-      <c r="B98" s="30"/>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="30"/>
+    <row r="98" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="33"/>
+      <c r="B98" s="33"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="33"/>
       <c r="G98" s="10" t="s">
         <v>136</v>
       </c>
@@ -6779,23 +6771,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="75.75" customHeight="1">
-      <c r="A99" s="30" t="s">
+    <row r="99" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B99" s="30" t="s">
+      <c r="B99" s="33" t="s">
         <v>295</v>
       </c>
-      <c r="C99" s="30" t="s">
+      <c r="C99" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D99" s="30" t="s">
+      <c r="D99" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="E99" s="30" t="s">
+      <c r="E99" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="F99" s="30" t="s">
+      <c r="F99" s="33" t="s">
         <v>297</v>
       </c>
       <c r="G99" s="10" t="s">
@@ -6820,13 +6812,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="75.75" customHeight="1">
-      <c r="A100" s="30"/>
-      <c r="B100" s="30"/>
-      <c r="C100" s="30"/>
-      <c r="D100" s="30"/>
-      <c r="E100" s="30"/>
-      <c r="F100" s="30"/>
+    <row r="100" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="33"/>
+      <c r="B100" s="33"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="33"/>
+      <c r="F100" s="33"/>
       <c r="G100" s="10" t="s">
         <v>136</v>
       </c>
@@ -6849,23 +6841,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="75.75" customHeight="1">
-      <c r="A101" s="30" t="s">
+    <row r="101" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B101" s="30" t="s">
+      <c r="B101" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="C101" s="30" t="s">
+      <c r="C101" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="D101" s="30" t="s">
+      <c r="D101" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="E101" s="30" t="s">
+      <c r="E101" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="F101" s="30" t="s">
+      <c r="F101" s="33" t="s">
         <v>299</v>
       </c>
       <c r="G101" s="10" t="s">
@@ -6890,13 +6882,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="75.75" customHeight="1">
-      <c r="A102" s="30"/>
-      <c r="B102" s="30"/>
-      <c r="C102" s="30"/>
-      <c r="D102" s="30"/>
-      <c r="E102" s="30"/>
-      <c r="F102" s="30"/>
+    <row r="102" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="33"/>
+      <c r="B102" s="33"/>
+      <c r="C102" s="33"/>
+      <c r="D102" s="33"/>
+      <c r="E102" s="33"/>
+      <c r="F102" s="33"/>
       <c r="G102" s="10" t="s">
         <v>136</v>
       </c>
@@ -6919,7 +6911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="74.650000000000006" customHeight="1">
+    <row r="103" spans="1:13" ht="74.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
         <v>300</v>
       </c>
@@ -6945,19 +6937,19 @@
       <c r="K103" s="10"/>
       <c r="L103" s="10"/>
     </row>
-    <row r="104" spans="1:13" ht="78" customHeight="1">
-      <c r="A104" s="30"/>
-      <c r="B104" s="30"/>
-      <c r="C104" s="30" t="s">
+    <row r="104" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="33"/>
+      <c r="B104" s="33"/>
+      <c r="C104" s="33" t="s">
         <v>304</v>
       </c>
-      <c r="D104" s="30" t="s">
+      <c r="D104" s="33" t="s">
         <v>305</v>
       </c>
-      <c r="E104" s="30" t="s">
+      <c r="E104" s="33" t="s">
         <v>306</v>
       </c>
-      <c r="F104" s="30" t="s">
+      <c r="F104" s="33" t="s">
         <v>307</v>
       </c>
       <c r="G104" s="10" t="s">
@@ -6977,13 +6969,13 @@
         <v>309</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="92.65" customHeight="1">
-      <c r="A105" s="30"/>
-      <c r="B105" s="30"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="30"/>
-      <c r="E105" s="30"/>
-      <c r="F105" s="30"/>
+    <row r="105" spans="1:13" ht="92.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="33"/>
+      <c r="B105" s="33"/>
+      <c r="C105" s="33"/>
+      <c r="D105" s="33"/>
+      <c r="E105" s="33"/>
+      <c r="F105" s="33"/>
       <c r="G105" s="10" t="s">
         <v>25</v>
       </c>
@@ -6999,19 +6991,19 @@
       <c r="K105" s="10"/>
       <c r="L105" s="10"/>
     </row>
-    <row r="106" spans="1:13" ht="49.5" customHeight="1">
-      <c r="A106" s="30"/>
-      <c r="B106" s="30"/>
-      <c r="C106" s="30" t="s">
+    <row r="106" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="33"/>
+      <c r="B106" s="33"/>
+      <c r="C106" s="33" t="s">
         <v>311</v>
       </c>
-      <c r="D106" s="30" t="s">
+      <c r="D106" s="33" t="s">
         <v>305</v>
       </c>
-      <c r="E106" s="30" t="s">
+      <c r="E106" s="33" t="s">
         <v>306</v>
       </c>
-      <c r="F106" s="30" t="s">
+      <c r="F106" s="33" t="s">
         <v>312</v>
       </c>
       <c r="G106" s="10" t="s">
@@ -7029,13 +7021,13 @@
       <c r="K106" s="10"/>
       <c r="L106" s="10"/>
     </row>
-    <row r="107" spans="1:13" ht="93.75" customHeight="1">
-      <c r="A107" s="30"/>
-      <c r="B107" s="30"/>
-      <c r="C107" s="30"/>
-      <c r="D107" s="30"/>
-      <c r="E107" s="30"/>
-      <c r="F107" s="30"/>
+    <row r="107" spans="1:13" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="33"/>
+      <c r="B107" s="33"/>
+      <c r="C107" s="33"/>
+      <c r="D107" s="33"/>
+      <c r="E107" s="33"/>
+      <c r="F107" s="33"/>
       <c r="G107" s="10" t="s">
         <v>25</v>
       </c>
@@ -7051,7 +7043,7 @@
       <c r="K107" s="10"/>
       <c r="L107" s="10"/>
     </row>
-    <row r="108" spans="1:13" ht="53.65" customHeight="1">
+    <row r="108" spans="1:13" ht="53.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
         <v>313</v>
       </c>
@@ -7090,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="53.65" customHeight="1">
+    <row r="109" spans="1:13" ht="53.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
         <v>319</v>
       </c>
@@ -7129,7 +7121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="75.75" customHeight="1">
+    <row r="110" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
         <v>324</v>
       </c>
@@ -7168,7 +7160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="75" customHeight="1">
+    <row r="111" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
         <v>329</v>
       </c>
@@ -7194,8 +7186,8 @@
       <c r="I111" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J111" s="10" t="s">
-        <v>423</v>
+      <c r="J111" s="27" t="s">
+        <v>437</v>
       </c>
       <c r="K111" s="10" t="s">
         <v>23</v>
@@ -7207,7 +7199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="75" customHeight="1">
+    <row r="112" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
         <v>153</v>
       </c>
@@ -7234,7 +7226,7 @@
         <v>21</v>
       </c>
       <c r="J112" s="10" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
       <c r="K112" s="10" t="s">
         <v>23</v>
@@ -7246,23 +7238,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="58.15" customHeight="1">
-      <c r="A113" s="30" t="s">
+    <row r="113" spans="1:13" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="33" t="s">
         <v>337</v>
       </c>
-      <c r="B113" s="30" t="s">
+      <c r="B113" s="33" t="s">
         <v>338</v>
       </c>
-      <c r="C113" s="30" t="s">
+      <c r="C113" s="33" t="s">
         <v>339</v>
       </c>
-      <c r="D113" s="30" t="s">
+      <c r="D113" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="E113" s="30" t="s">
+      <c r="E113" s="33" t="s">
         <v>340</v>
       </c>
-      <c r="F113" s="30" t="s">
+      <c r="F113" s="33" t="s">
         <v>341</v>
       </c>
       <c r="G113" s="10" t="s">
@@ -7287,13 +7279,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="60">
-      <c r="A114" s="30"/>
-      <c r="B114" s="30"/>
-      <c r="C114" s="30"/>
-      <c r="D114" s="30"/>
-      <c r="E114" s="30"/>
-      <c r="F114" s="30"/>
+    <row r="114" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A114" s="33"/>
+      <c r="B114" s="33"/>
+      <c r="C114" s="33"/>
+      <c r="D114" s="33"/>
+      <c r="E114" s="33"/>
+      <c r="F114" s="33"/>
       <c r="G114" s="10" t="s">
         <v>25</v>
       </c>
@@ -7316,12 +7308,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="49.5" customHeight="1">
-      <c r="A115" s="30"/>
-      <c r="B115" s="30"/>
-      <c r="C115" s="30"/>
-      <c r="D115" s="30"/>
-      <c r="E115" s="30"/>
+    <row r="115" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="33"/>
+      <c r="B115" s="33"/>
+      <c r="C115" s="33"/>
+      <c r="D115" s="33"/>
+      <c r="E115" s="33"/>
       <c r="F115" s="10" t="s">
         <v>343</v>
       </c>
@@ -7335,7 +7327,7 @@
         <v>137</v>
       </c>
       <c r="J115" s="10" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="K115" s="10" t="s">
         <v>23</v>
@@ -7347,17 +7339,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="96.6" customHeight="1">
-      <c r="A116" s="30"/>
-      <c r="B116" s="30"/>
-      <c r="C116" s="30" t="s">
+    <row r="116" spans="1:13" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="33"/>
+      <c r="B116" s="33"/>
+      <c r="C116" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="D116" s="30" t="s">
+      <c r="D116" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="E116" s="30"/>
-      <c r="F116" s="31" t="s">
+      <c r="E116" s="33"/>
+      <c r="F116" s="42" t="s">
         <v>345</v>
       </c>
       <c r="G116" s="10" t="s">
@@ -7375,13 +7367,13 @@
       <c r="K116" s="10"/>
       <c r="L116" s="10"/>
     </row>
-    <row r="117" spans="1:13" ht="96.6" customHeight="1">
-      <c r="A117" s="30"/>
-      <c r="B117" s="30"/>
-      <c r="C117" s="30"/>
-      <c r="D117" s="30"/>
-      <c r="E117" s="30"/>
-      <c r="F117" s="31"/>
+    <row r="117" spans="1:13" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="33"/>
+      <c r="B117" s="33"/>
+      <c r="C117" s="33"/>
+      <c r="D117" s="33"/>
+      <c r="E117" s="33"/>
+      <c r="F117" s="42"/>
       <c r="G117" s="10" t="s">
         <v>25</v>
       </c>
@@ -7399,15 +7391,15 @@
       </c>
       <c r="L117" s="10"/>
     </row>
-    <row r="118" spans="1:13" ht="42" customHeight="1">
-      <c r="A118" s="30"/>
-      <c r="B118" s="30"/>
-      <c r="C118" s="30"/>
-      <c r="D118" s="30" t="s">
+    <row r="118" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="33"/>
+      <c r="B118" s="33"/>
+      <c r="C118" s="33"/>
+      <c r="D118" s="33" t="s">
         <v>348</v>
       </c>
-      <c r="E118" s="30"/>
-      <c r="F118" s="31" t="s">
+      <c r="E118" s="33"/>
+      <c r="F118" s="42" t="s">
         <v>349</v>
       </c>
       <c r="G118" s="10" t="s">
@@ -7430,13 +7422,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A119" s="30"/>
-      <c r="B119" s="30"/>
-      <c r="C119" s="30"/>
-      <c r="D119" s="30"/>
-      <c r="E119" s="30"/>
-      <c r="F119" s="31"/>
+    <row r="119" spans="1:13" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="33"/>
+      <c r="B119" s="33"/>
+      <c r="C119" s="33"/>
+      <c r="D119" s="33"/>
+      <c r="E119" s="33"/>
+      <c r="F119" s="42"/>
       <c r="G119" s="10" t="s">
         <v>25</v>
       </c>
@@ -7459,7 +7451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="30">
+    <row r="120" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10" t="s">
@@ -7487,17 +7479,17 @@
       <c r="K120" s="10"/>
       <c r="L120" s="10"/>
     </row>
-    <row r="121" spans="1:13" ht="99" customHeight="1" thickTop="1">
-      <c r="A121" s="30"/>
-      <c r="B121" s="30"/>
-      <c r="C121" s="30" t="s">
+    <row r="121" spans="1:13" ht="99" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="33"/>
+      <c r="B121" s="33"/>
+      <c r="C121" s="33" t="s">
         <v>355</v>
       </c>
-      <c r="D121" s="30" t="s">
+      <c r="D121" s="33" t="s">
         <v>355</v>
       </c>
-      <c r="E121" s="30"/>
-      <c r="F121" s="38" t="s">
+      <c r="E121" s="33"/>
+      <c r="F121" s="36" t="s">
         <v>356</v>
       </c>
       <c r="G121" s="10" t="s">
@@ -7515,13 +7507,13 @@
       <c r="K121" s="10"/>
       <c r="L121" s="10"/>
     </row>
-    <row r="122" spans="1:13" ht="99" customHeight="1">
-      <c r="A122" s="30"/>
-      <c r="B122" s="30"/>
-      <c r="C122" s="30"/>
-      <c r="D122" s="30"/>
-      <c r="E122" s="30"/>
-      <c r="F122" s="38"/>
+    <row r="122" spans="1:13" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="33"/>
+      <c r="B122" s="33"/>
+      <c r="C122" s="33"/>
+      <c r="D122" s="33"/>
+      <c r="E122" s="33"/>
+      <c r="F122" s="36"/>
       <c r="G122" s="10" t="s">
         <v>25</v>
       </c>
@@ -7537,12 +7529,12 @@
       <c r="K122" s="10"/>
       <c r="L122" s="10"/>
     </row>
-    <row r="123" spans="1:13" ht="43.9" customHeight="1">
-      <c r="A123" s="30"/>
-      <c r="B123" s="30"/>
-      <c r="C123" s="30"/>
-      <c r="D123" s="30"/>
-      <c r="E123" s="30"/>
+    <row r="123" spans="1:13" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="33"/>
+      <c r="B123" s="33"/>
+      <c r="C123" s="33"/>
+      <c r="D123" s="33"/>
+      <c r="E123" s="33"/>
       <c r="F123" s="12" t="s">
         <v>359</v>
       </c>
@@ -7561,12 +7553,12 @@
       <c r="K123" s="10"/>
       <c r="L123" s="10"/>
     </row>
-    <row r="124" spans="1:13" ht="84" customHeight="1">
-      <c r="A124" s="30"/>
-      <c r="B124" s="30"/>
-      <c r="C124" s="30"/>
-      <c r="D124" s="30"/>
-      <c r="E124" s="30"/>
+    <row r="124" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="33"/>
+      <c r="B124" s="33"/>
+      <c r="C124" s="33"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="33"/>
       <c r="F124" s="12" t="s">
         <v>361</v>
       </c>
@@ -7579,11 +7571,11 @@
       <c r="K124" s="10"/>
       <c r="L124" s="10"/>
     </row>
-    <row r="125" spans="1:13" ht="106.9" customHeight="1">
-      <c r="A125" s="30"/>
-      <c r="B125" s="30"/>
-      <c r="C125" s="30"/>
-      <c r="D125" s="30"/>
+    <row r="125" spans="1:13" ht="106.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="33"/>
+      <c r="B125" s="33"/>
+      <c r="C125" s="33"/>
+      <c r="D125" s="33"/>
       <c r="E125" s="32" t="s">
         <v>363</v>
       </c>
@@ -7607,11 +7599,11 @@
       </c>
       <c r="L125" s="10"/>
     </row>
-    <row r="126" spans="1:13" ht="106.9" customHeight="1">
-      <c r="A126" s="30"/>
-      <c r="B126" s="30"/>
-      <c r="C126" s="30"/>
-      <c r="D126" s="30"/>
+    <row r="126" spans="1:13" ht="106.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="33"/>
+      <c r="B126" s="33"/>
+      <c r="C126" s="33"/>
+      <c r="D126" s="33"/>
       <c r="E126" s="32"/>
       <c r="F126" s="32"/>
       <c r="G126" s="7" t="s">
@@ -7629,11 +7621,11 @@
       <c r="K126" s="10"/>
       <c r="L126" s="10"/>
     </row>
-    <row r="127" spans="1:13" ht="60">
-      <c r="A127" s="30"/>
-      <c r="B127" s="30"/>
-      <c r="C127" s="30"/>
-      <c r="D127" s="30"/>
+    <row r="127" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A127" s="33"/>
+      <c r="B127" s="33"/>
+      <c r="C127" s="33"/>
+      <c r="D127" s="33"/>
       <c r="E127" s="32" t="s">
         <v>368</v>
       </c>
@@ -7662,11 +7654,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="167.25" customHeight="1">
-      <c r="A128" s="30"/>
-      <c r="B128" s="30"/>
-      <c r="C128" s="30"/>
-      <c r="D128" s="30"/>
+    <row r="128" spans="1:13" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="33"/>
+      <c r="B128" s="33"/>
+      <c r="C128" s="33"/>
+      <c r="D128" s="33"/>
       <c r="E128" s="32"/>
       <c r="F128" s="32"/>
       <c r="G128" s="7" t="s">
@@ -7691,10 +7683,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="76.150000000000006" customHeight="1">
-      <c r="A129" s="30"/>
-      <c r="B129" s="30"/>
-      <c r="C129" s="30"/>
+    <row r="129" spans="1:13" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="33"/>
+      <c r="B129" s="33"/>
+      <c r="C129" s="33"/>
       <c r="D129" s="10" t="s">
         <v>372</v>
       </c>
@@ -7719,10 +7711,10 @@
       <c r="K129" s="10"/>
       <c r="L129" s="10"/>
     </row>
-    <row r="130" spans="1:13" ht="46.9" customHeight="1">
-      <c r="A130" s="30"/>
-      <c r="B130" s="30"/>
-      <c r="C130" s="30"/>
+    <row r="130" spans="1:13" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="33"/>
+      <c r="B130" s="33"/>
+      <c r="C130" s="33"/>
       <c r="D130" s="10" t="s">
         <v>375</v>
       </c>
@@ -7747,10 +7739,10 @@
       <c r="K130" s="10"/>
       <c r="L130" s="10"/>
     </row>
-    <row r="131" spans="1:13" ht="177.75" customHeight="1">
-      <c r="A131" s="30"/>
-      <c r="B131" s="30"/>
-      <c r="C131" s="30"/>
+    <row r="131" spans="1:13" ht="177.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="33"/>
+      <c r="B131" s="33"/>
+      <c r="C131" s="33"/>
       <c r="D131" s="10" t="s">
         <v>377</v>
       </c>
@@ -7775,10 +7767,10 @@
       <c r="K131" s="10"/>
       <c r="L131" s="10"/>
     </row>
-    <row r="132" spans="1:13" ht="123.6" customHeight="1">
-      <c r="A132" s="30"/>
-      <c r="B132" s="30"/>
-      <c r="C132" s="30"/>
+    <row r="132" spans="1:13" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="33"/>
+      <c r="B132" s="33"/>
+      <c r="C132" s="33"/>
       <c r="D132" s="10" t="s">
         <v>380</v>
       </c>
@@ -7803,7 +7795,7 @@
       <c r="K132" s="10"/>
       <c r="L132" s="10"/>
     </row>
-    <row r="133" spans="1:13" ht="95.65" customHeight="1">
+    <row r="133" spans="1:13" ht="95.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7" t="s">
@@ -7840,7 +7832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="92.45" customHeight="1">
+    <row r="134" spans="1:13" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>390</v>
       </c>
@@ -7869,7 +7861,7 @@
         <v>137</v>
       </c>
       <c r="J134" s="7" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K134" s="18" t="s">
         <v>395</v>
@@ -7881,7 +7873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -7893,7 +7885,7 @@
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -7905,7 +7897,7 @@
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="8"/>
       <c r="B162" s="37" t="s">
         <v>396</v>
@@ -7921,42 +7913,212 @@
     </row>
   </sheetData>
   <mergeCells count="271">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="B22:B35"/>
-    <mergeCell ref="C22:C35"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="C121:C132"/>
-    <mergeCell ref="B121:B132"/>
-    <mergeCell ref="A121:A132"/>
-    <mergeCell ref="E121:E124"/>
-    <mergeCell ref="D121:D128"/>
-    <mergeCell ref="E127:E128"/>
-    <mergeCell ref="F127:F128"/>
-    <mergeCell ref="E125:E126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="F121:F122"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="F101:F102"/>
-    <mergeCell ref="E101:E102"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="F95:F96"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="C116:C119"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="C113:C115"/>
+    <mergeCell ref="B113:B115"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="E99:E100"/>
+    <mergeCell ref="F99:F100"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="D95:D96"/>
+    <mergeCell ref="E95:E96"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
     <mergeCell ref="B162:J162"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -7981,217 +8143,47 @@
     <mergeCell ref="D79:D80"/>
     <mergeCell ref="E79:E80"/>
     <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="F101:F102"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="F95:F96"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="C121:C132"/>
+    <mergeCell ref="B121:B132"/>
+    <mergeCell ref="A121:A132"/>
+    <mergeCell ref="E121:E124"/>
+    <mergeCell ref="D121:D128"/>
+    <mergeCell ref="E127:E128"/>
+    <mergeCell ref="F127:F128"/>
+    <mergeCell ref="E125:E126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="F121:F122"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B22:B35"/>
+    <mergeCell ref="C22:C35"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F28:F29"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="D95:D96"/>
-    <mergeCell ref="E95:E96"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="E99:E100"/>
-    <mergeCell ref="F99:F100"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="C116:C119"/>
-    <mergeCell ref="F113:F114"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="C113:C115"/>
-    <mergeCell ref="B113:B115"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="B116:B119"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="K3">
@@ -8254,7 +8246,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2 K10 K47 K49 K58:K59 K61 K63:K64 K68 K71 K73 K82 K84 K86 K88 K90 K92 K94 K124:K125 K133:K135 K137 K139 K66 K6 K96:K102 K120:L120 K116:L117">
+  <conditionalFormatting sqref="K10 K2 K47 K49 K58:K59 K61 K63:K64 K68 K71 K73 K82 K84 K86 K88 K90 K92 K94 K124:K125 K133:K135 K137 K139 K66 K6 K96:K102 K120:L120 K116:L117">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -8278,7 +8270,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K106 K104">
+  <conditionalFormatting sqref="K104 K106">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -8350,7 +8342,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2 L10 L47 L49 L58:L59 L61 L68 L82 L84 L86 L88 L90 L92 L94 L124:L125 L133:L135 L137 L139 L6 L96:L102 L71:L73 L63:L66">
+  <conditionalFormatting sqref="L10 L2 L47 L49 L58:L59 L61 L68 L82 L84 L86 L88 L90 L92 L94 L124:L125 L133:L135 L137 L139 L6 L96:L102 L71:L73 L63:L66">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -8398,7 +8390,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L106 L104">
+  <conditionalFormatting sqref="L104 L106">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -8547,14 +8539,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -8567,7 +8559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -8578,7 +8570,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>398</v>
       </c>
@@ -8589,7 +8581,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -8600,7 +8592,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>400</v>
       </c>
@@ -8611,7 +8603,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -8619,7 +8611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>402</v>
       </c>
@@ -8641,49 +8633,49 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>411</v>
       </c>

</xml_diff>